<commit_message>
Filtro de preço implementado e alteração na planilha
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27031"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ProjetosPython\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E44DFE-809C-4E2C-AA3C-CC007216EA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B02D8CD-025F-468E-B418-F5A6FD40B0E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="4260" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7575" yWindow="4605" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Preço máximo</t>
   </si>
   <si>
-    <t>iphone 12 64gb</t>
-  </si>
-  <si>
     <t>mini watch</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>galax</t>
+  </si>
+  <si>
+    <t>iphone 12 64 gb</t>
   </si>
 </sst>
 </file>
@@ -84,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +370,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,10 +391,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>3000</v>
@@ -403,11 +404,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>1800</v>

</xml_diff>

<commit_message>
Ajustes novos para Buscape
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ProjetosPython\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F29861E-BF67-4DB1-9848-35B3A9EABE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4AE967-6772-44E0-B51B-61A693760832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4200" yWindow="2085" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +413,7 @@
         <v>1800</v>
       </c>
       <c r="D3">
-        <v>2500</v>
+        <v>3500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>